<commit_message>
Updated Burndown Chart and Scrum Board
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint3/Burndown chart.xlsx
+++ b/Project_Management/Sprint3/Burndown chart.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\ES2324\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\ES2324\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F7676A-AB17-4204-9F4F-8280F79F0E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBF7890-0C6F-413B-A6C9-7FA02F00AB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -659,6 +659,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,15 +712,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,7 +738,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -843,7 +840,7 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -960,22 +957,22 @@
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,7 +2231,7 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,52 +2247,52 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="50"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="53"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2332,8 +2329,8 @@
       <c r="S4" s="5"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2368,7 @@
       <c r="B6" s="30">
         <v>1</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="33">
@@ -2406,7 +2403,9 @@
       <c r="E7" s="13">
         <v>2</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -2484,7 +2483,9 @@
         <v>5</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14">
+        <v>2</v>
+      </c>
       <c r="G10" s="37"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2503,13 +2504,13 @@
       <c r="B11" s="31">
         <v>6</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="35">
         <v>2</v>
       </c>
-      <c r="E11" s="56"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -2535,10 +2536,12 @@
       <c r="D12" s="35">
         <v>3</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="19">
         <v>0.5</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2579,7 +2582,7 @@
       <c r="B14" s="31">
         <v>9</v>
       </c>
-      <c r="C14" s="55"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="35"/>
       <c r="E14" s="19"/>
       <c r="F14" s="14"/>
@@ -2708,10 +2711,10 @@
       <c r="S19" s="16"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="3">
         <v>0</v>
       </c>
@@ -2721,7 +2724,7 @@
       </c>
       <c r="F20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="21">
         <f t="shared" si="0"/>
@@ -2754,10 +2757,10 @@
       <c r="T20" s="29"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="24">
         <f>SUM(D6:D20)</f>
         <v>20</v>
@@ -2768,27 +2771,27 @@
       </c>
       <c r="F21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="H21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -2800,10 +2803,10 @@
       <c r="S21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="26">
         <f>D21</f>
         <v>20</v>

</xml_diff>

<commit_message>
uploaded final burndown chart and scrum board
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint3/Burndown chart.xlsx
+++ b/Project_Management/Sprint3/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\ES2324\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0CEA64-9F06-4CA8-AE0B-438132DB3C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6190EF97-5CCB-4DE2-83F0-D08EF97D7649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,18 +199,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -555,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -663,23 +651,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -729,8 +708,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,10 +853,10 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,10 +970,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,7 +2232,7 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,52 +2248,52 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="53"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="50"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="56"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="53"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2348,8 +2330,8 @@
       <c r="S4" s="5"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="46"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2384,10 +2366,10 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="41">
+      <c r="B6" s="57">
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="56" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="32">
@@ -2398,8 +2380,12 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -2410,7 +2396,7 @@
       <c r="S6" s="12"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="42">
+      <c r="B7" s="38">
         <v>2</v>
       </c>
       <c r="C7" s="37" t="s">
@@ -2428,7 +2414,9 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="14">
+        <v>1</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
@@ -2440,10 +2428,10 @@
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="39">
+      <c r="B8" s="38">
         <v>3</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="33">
@@ -2470,10 +2458,10 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="39">
+      <c r="B9" s="38">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="33">
@@ -2498,10 +2486,10 @@
       <c r="S9" s="16"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="39">
+      <c r="B10" s="38">
         <v>5</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="34">
@@ -2528,10 +2516,10 @@
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="39">
+      <c r="B11" s="38">
         <v>6</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="34">
@@ -2560,10 +2548,10 @@
       <c r="S11" s="16"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="39">
+      <c r="B12" s="38">
         <v>7</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="37" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="34">
@@ -2596,10 +2584,10 @@
       <c r="S12" s="16"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="39">
+      <c r="B13" s="38">
         <v>8</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="34">
@@ -2758,10 +2746,10 @@
       <c r="S19" s="16"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="3">
         <v>0</v>
       </c>
@@ -2787,11 +2775,11 @@
       </c>
       <c r="J20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2804,10 +2792,10 @@
       <c r="T20" s="29"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="24">
         <f>SUM(D6:D20)</f>
         <v>20</v>
@@ -2834,11 +2822,11 @@
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -2850,10 +2838,10 @@
       <c r="S21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="50"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="26">
         <f>D21</f>
         <v>20</v>

</xml_diff>